<commit_message>
Changed Linearization to use B[t] and corrected bug
</commit_message>
<xml_diff>
--- a/linearization_heuristic_dyn_models/linearization_heuristic_results_10_days.xlsx
+++ b/linearization_heuristic_dyn_models/linearization_heuristic_results_10_days.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,40 +452,45 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>eta</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>heuristic</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>icus</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>lockdown_freq</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>reward</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>test_freq</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>testing</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>tests</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>xi</t>
         </is>
@@ -496,41 +501,44 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>574.0756800992668</v>
+        <v>1604.768326474094</v>
       </c>
       <c r="C2" t="n">
         <v>0.5</v>
       </c>
       <c r="D2" t="n">
-        <v>5785478732.774339</v>
-      </c>
-      <c r="E2" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F2" t="inlineStr">
         <is>
           <t>linearization_heuristic</t>
         </is>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>3000</v>
       </c>
-      <c r="G2" t="n">
-        <v>14</v>
-      </c>
       <c r="H2" t="n">
-        <v>5192001427.49943</v>
+        <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>7</v>
-      </c>
-      <c r="J2" t="inlineStr">
+        <v>-2320349377.127979</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t>linearization_heuristic</t>
         </is>
       </c>
-      <c r="K2" t="n">
-        <v>30000</v>
-      </c>
       <c r="L2" t="n">
-        <v>1000000</v>
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1115970.9</v>
       </c>
     </row>
     <row r="3">
@@ -538,41 +546,44 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>491.4048706061304</v>
+        <v>1604.768326474094</v>
       </c>
       <c r="C3" t="n">
         <v>0.5</v>
       </c>
       <c r="D3" t="n">
-        <v>5785478732.774339</v>
-      </c>
-      <c r="E3" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F3" t="inlineStr">
         <is>
           <t>linearization_heuristic_Prop_Bouncing</t>
         </is>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>3000</v>
       </c>
-      <c r="G3" t="n">
-        <v>14</v>
-      </c>
       <c r="H3" t="n">
-        <v>5274672236.992566</v>
+        <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>7</v>
-      </c>
-      <c r="J3" t="inlineStr">
+        <v>-2320349377.127979</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" t="inlineStr">
         <is>
           <t>linearization_heuristic</t>
         </is>
       </c>
-      <c r="K3" t="n">
-        <v>30000</v>
-      </c>
       <c r="L3" t="n">
-        <v>1000000</v>
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>1115970.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed linearization to use beta[t]
</commit_message>
<xml_diff>
--- a/linearization_heuristic_dyn_models/linearization_heuristic_results_10_days.xlsx
+++ b/linearization_heuristic_dyn_models/linearization_heuristic_results_10_days.xlsx
@@ -501,13 +501,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1604.768326474094</v>
+        <v>0.2100747399255385</v>
       </c>
       <c r="C2" t="n">
         <v>0.5</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>5888186138.283437</v>
       </c>
       <c r="E2" t="n">
         <v>0.1</v>
@@ -518,13 +518,13 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>3000</v>
+        <v>0.3</v>
       </c>
       <c r="H2" t="n">
         <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>-2320349377.127979</v>
+        <v>2850696028.994353</v>
       </c>
       <c r="J2" t="n">
         <v>1</v>
@@ -538,7 +538,7 @@
         <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>1115970.9</v>
+        <v>11159709000</v>
       </c>
     </row>
     <row r="3">
@@ -546,13 +546,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1604.768326474094</v>
+        <v>0.2100747399255385</v>
       </c>
       <c r="C3" t="n">
         <v>0.5</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>5888186138.283437</v>
       </c>
       <c r="E3" t="n">
         <v>0.1</v>
@@ -563,13 +563,13 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>3000</v>
+        <v>0.3</v>
       </c>
       <c r="H3" t="n">
         <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>-2320349377.127979</v>
+        <v>2850696028.994353</v>
       </c>
       <c r="J3" t="n">
         <v>1</v>
@@ -583,7 +583,7 @@
         <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>1115970.9</v>
+        <v>11159709000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>